<commit_message>
Updated compiled survey raw data
</commit_message>
<xml_diff>
--- a/documents/resources/evaluation/usability/Survey-Compiled.xlsx
+++ b/documents/resources/evaluation/usability/Survey-Compiled.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="540" windowWidth="24880" windowHeight="16740" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="2640" yWindow="540" windowWidth="24880" windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
     <sheet name="Demographic" sheetId="3" r:id="rId2"/>
     <sheet name="Scenario 1" sheetId="2" r:id="rId3"/>
     <sheet name="Scenario 2" sheetId="4" r:id="rId4"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="163">
   <si>
     <t>Male</t>
   </si>
@@ -500,13 +500,28 @@
   </si>
   <si>
     <t>SCORE</t>
+  </si>
+  <si>
+    <t>TAKEN OUT BECAUSE RESPONDENT SKIP BOTH SCENARIO</t>
+  </si>
+  <si>
+    <t>I am not sure. I am stuck at instruction number 3. It says filetype not supported, So I cannot proceed to the next step after submitting the config and geometry files.</t>
+  </si>
+  <si>
+    <t>I could not run the program (It says: fail to download simulation information from URL)</t>
+  </si>
+  <si>
+    <t>It doesn't seem to work (Maybe due to firewall? I am not sure)</t>
+  </si>
+  <si>
+    <t>It might be quite easy to work (If it works)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -535,8 +550,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -546,6 +566,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -559,7 +585,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -663,22 +689,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -730,6 +762,8 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -781,6 +815,8 @@
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -803,7 +839,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -895,7 +930,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1045,7 +1079,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1271,11 +1304,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2130654536"/>
-        <c:axId val="-2130191016"/>
+        <c:axId val="-2120135224"/>
+        <c:axId val="-2125396568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130654536"/>
+        <c:axId val="-2120135224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1284,7 +1317,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130191016"/>
+        <c:crossAx val="-2125396568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1292,7 +1325,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130191016"/>
+        <c:axId val="-2125396568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1303,14 +1336,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130654536"/>
+        <c:crossAx val="-2120135224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1340,7 +1372,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1422,11 +1453,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2144724568"/>
-        <c:axId val="2123073608"/>
+        <c:axId val="-2146272408"/>
+        <c:axId val="-2121452936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2144724568"/>
+        <c:axId val="-2146272408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1435,7 +1466,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123073608"/>
+        <c:crossAx val="-2121452936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1443,7 +1474,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123073608"/>
+        <c:axId val="-2121452936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1454,14 +1485,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144724568"/>
+        <c:crossAx val="-2146272408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1491,7 +1521,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1567,11 +1596,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2127681896"/>
-        <c:axId val="-2124483592"/>
+        <c:axId val="-2121649720"/>
+        <c:axId val="-2139851400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2127681896"/>
+        <c:axId val="-2121649720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1580,7 +1609,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124483592"/>
+        <c:crossAx val="-2139851400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1588,7 +1617,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124483592"/>
+        <c:axId val="-2139851400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1599,14 +1628,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127681896"/>
+        <c:crossAx val="-2121649720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1882,11 +1910,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2119497656"/>
-        <c:axId val="-2119688936"/>
+        <c:axId val="-2126847544"/>
+        <c:axId val="-2127720984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2119497656"/>
+        <c:axId val="-2126847544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1895,7 +1923,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119688936"/>
+        <c:crossAx val="-2127720984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1903,7 +1931,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2119688936"/>
+        <c:axId val="-2127720984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1914,7 +1942,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119497656"/>
+        <c:crossAx val="-2126847544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2033,11 +2061,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2131824952"/>
-        <c:axId val="-2140649288"/>
+        <c:axId val="-2140129896"/>
+        <c:axId val="-2143278152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2131824952"/>
+        <c:axId val="-2140129896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2046,7 +2074,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140649288"/>
+        <c:crossAx val="-2143278152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2054,7 +2082,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2140649288"/>
+        <c:axId val="-2143278152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2065,7 +2093,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2131824952"/>
+        <c:crossAx val="-2140129896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2178,11 +2206,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2120415256"/>
-        <c:axId val="-2120440408"/>
+        <c:axId val="-2124762152"/>
+        <c:axId val="-2139958632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2120415256"/>
+        <c:axId val="-2124762152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2191,7 +2219,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120440408"/>
+        <c:crossAx val="-2139958632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2199,7 +2227,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2120440408"/>
+        <c:axId val="-2139958632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2210,7 +2238,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120415256"/>
+        <c:crossAx val="-2124762152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2815,8 +2843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ23"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4933,17 +4961,150 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:43">
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
+    <row r="22" spans="1:43">
+      <c r="A22" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:43" ht="16">
+      <c r="A23" s="6">
+        <v>42498.708854166667</v>
+      </c>
+      <c r="B23" s="7">
+        <v>32</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="7">
+        <v>2</v>
+      </c>
+      <c r="G23" s="7">
+        <v>5</v>
+      </c>
+      <c r="H23" s="7">
+        <v>1</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="N23" s="7">
+        <v>1</v>
+      </c>
+      <c r="O23" s="7">
+        <v>3</v>
+      </c>
+      <c r="P23" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="T23" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="U23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="V23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="W23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="X23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN23" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="AO23" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="AP23" s="7">
+        <v>1</v>
+      </c>
+      <c r="AQ23" s="7">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="L23:Q23"/>
+    <mergeCell ref="A22:F22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4975,7 +5136,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <f>COUNTIF(Sheet1!C2:C17, "Male")</f>
+        <f>COUNTIF('Raw Data'!C2:C17, "Male")</f>
         <v>14</v>
       </c>
     </row>
@@ -4984,7 +5145,7 @@
         <v>28</v>
       </c>
       <c r="C4">
-        <f>COUNTIF(Sheet1!C2:C17, "Female")</f>
+        <f>COUNTIF('Raw Data'!C2:C17, "Female")</f>
         <v>1</v>
       </c>
     </row>
@@ -4998,7 +5159,7 @@
         <v>108</v>
       </c>
       <c r="C22">
-        <f>COUNTIF(Sheet1!$D$2:$D$17, "MSc student")</f>
+        <f>COUNTIF('Raw Data'!$D$2:$D$17, "MSc student")</f>
         <v>7</v>
       </c>
     </row>
@@ -5007,7 +5168,7 @@
         <v>109</v>
       </c>
       <c r="C23">
-        <f>COUNTIF(Sheet1!$D$2:$D$17, "PhD student")</f>
+        <f>COUNTIF('Raw Data'!$D$2:$D$17, "PhD student")</f>
         <v>2</v>
       </c>
     </row>
@@ -5016,7 +5177,7 @@
         <v>29</v>
       </c>
       <c r="C24">
-        <f>COUNTIF(Sheet1!$D$2:$D$17, "PDRA")</f>
+        <f>COUNTIF('Raw Data'!$D$2:$D$17, "PDRA")</f>
         <v>1</v>
       </c>
     </row>
@@ -5025,7 +5186,7 @@
         <v>13</v>
       </c>
       <c r="C25">
-        <f>COUNTIF(Sheet1!$D$2:$D$17, "Lecturer")</f>
+        <f>COUNTIF('Raw Data'!$D$2:$D$17, "Lecturer")</f>
         <v>1</v>
       </c>
     </row>
@@ -5034,7 +5195,7 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <f>COUNTIF(Sheet1!$D$2:$D$17, "Professor")</f>
+        <f>COUNTIF('Raw Data'!$D$2:$D$17, "Professor")</f>
         <v>1</v>
       </c>
     </row>
@@ -5043,7 +5204,7 @@
         <v>40</v>
       </c>
       <c r="C27">
-        <f>COUNTIF(Sheet1!$D$2:$D$17, "Professional")</f>
+        <f>COUNTIF('Raw Data'!$D$2:$D$17, "Professional")</f>
         <v>1</v>
       </c>
     </row>
@@ -5116,29 +5277,29 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <f>COUNTIF(Sheet1!J$2:J$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!J$2:J$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f>COUNTIF(Sheet1!K$2:K$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!K$2:K$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f>COUNTIF(Sheet1!L$2:L$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!L$2:L$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="G4" t="s">
         <v>117</v>
       </c>
       <c r="H4">
-        <f>COUNTIF(Sheet1!N$2:$N17, 1)</f>
+        <f>COUNTIF('Raw Data'!N$2:$N17, 1)</f>
         <v>1</v>
       </c>
       <c r="I4" t="s">
         <v>113</v>
       </c>
       <c r="J4">
-        <f>COUNTIF(Sheet1!O$2:O$17, 1)</f>
+        <f>COUNTIF('Raw Data'!O$2:O$17, 1)</f>
         <v>6</v>
       </c>
     </row>
@@ -5147,29 +5308,29 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <f>COUNTIF(Sheet1!J$2:J$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!J$2:J$17, "Disagree")</f>
         <v>0</v>
       </c>
       <c r="D5">
-        <f>COUNTIF(Sheet1!K$2:K$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!K$2:K$17, "Disagree")</f>
         <v>0</v>
       </c>
       <c r="E5">
-        <f>COUNTIF(Sheet1!L$2:L$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!L$2:L$17, "Disagree")</f>
         <v>0</v>
       </c>
       <c r="G5" t="s">
         <v>118</v>
       </c>
       <c r="H5">
-        <f>COUNTIF(Sheet1!N$2:$N18, 2)</f>
+        <f>COUNTIF('Raw Data'!N$2:$N18, 2)</f>
         <v>3</v>
       </c>
       <c r="I5" t="s">
         <v>115</v>
       </c>
       <c r="J5">
-        <f>COUNTIF(Sheet1!O$2:O$17, 2)</f>
+        <f>COUNTIF('Raw Data'!O$2:O$17, 2)</f>
         <v>2</v>
       </c>
     </row>
@@ -5178,29 +5339,29 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <f>COUNTIF(Sheet1!J$2:J$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!J$2:J$17, "Neutral")</f>
         <v>2</v>
       </c>
       <c r="D6">
-        <f>COUNTIF(Sheet1!K$2:K$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!K$2:K$17, "Neutral")</f>
         <v>2</v>
       </c>
       <c r="E6">
-        <f>COUNTIF(Sheet1!L$2:L$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!L$2:L$17, "Neutral")</f>
         <v>3</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
       </c>
       <c r="H6">
-        <f>COUNTIF(Sheet1!N$2:$N19, 3)</f>
+        <f>COUNTIF('Raw Data'!N$2:$N19, 3)</f>
         <v>4</v>
       </c>
       <c r="I6" t="s">
         <v>116</v>
       </c>
       <c r="J6">
-        <f>COUNTIF(Sheet1!O$2:O$17, 3)</f>
+        <f>COUNTIF('Raw Data'!O$2:O$17, 3)</f>
         <v>6</v>
       </c>
     </row>
@@ -5209,29 +5370,29 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <f>COUNTIF(Sheet1!J$2:J$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!J$2:J$17, "Agree")</f>
         <v>5</v>
       </c>
       <c r="D7">
-        <f>COUNTIF(Sheet1!K$2:K$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!K$2:K$17, "Agree")</f>
         <v>5</v>
       </c>
       <c r="E7">
-        <f>COUNTIF(Sheet1!L$2:L$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!L$2:L$17, "Agree")</f>
         <v>4</v>
       </c>
       <c r="G7" t="s">
         <v>119</v>
       </c>
       <c r="H7">
-        <f>COUNTIF(Sheet1!N$2:$N20, 4)</f>
+        <f>COUNTIF('Raw Data'!N$2:$N20, 4)</f>
         <v>2</v>
       </c>
       <c r="I7" t="s">
         <v>114</v>
       </c>
       <c r="J7">
-        <f>COUNTIF(Sheet1!O$2:O$17, 4)</f>
+        <f>COUNTIF('Raw Data'!O$2:O$17, 4)</f>
         <v>1</v>
       </c>
     </row>
@@ -5240,22 +5401,22 @@
         <v>15</v>
       </c>
       <c r="C8">
-        <f>COUNTIF(Sheet1!J$2:J$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!J$2:J$17, "Strongly agree")</f>
         <v>8</v>
       </c>
       <c r="D8">
-        <f>COUNTIF(Sheet1!K$2:K$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!K$2:K$17, "Strongly agree")</f>
         <v>8</v>
       </c>
       <c r="E8">
-        <f>COUNTIF(Sheet1!L$2:L$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!L$2:L$17, "Strongly agree")</f>
         <v>7</v>
       </c>
       <c r="G8" t="s">
         <v>120</v>
       </c>
       <c r="H8">
-        <f>COUNTIF(Sheet1!N$2:$N21, 5)</f>
+        <f>COUNTIF('Raw Data'!N$2:$N21, 5)</f>
         <v>5</v>
       </c>
     </row>
@@ -5264,15 +5425,15 @@
         <v>112</v>
       </c>
       <c r="C9">
-        <f>COUNTIF(Sheet1!J$2:J$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!J$2:J$17, "Not Applicable")</f>
         <v>0</v>
       </c>
       <c r="D9">
-        <f>COUNTIF(Sheet1!K$2:K$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!K$2:K$17, "Not Applicable")</f>
         <v>0</v>
       </c>
       <c r="E9">
-        <f>COUNTIF(Sheet1!L$2:L$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!L$2:L$17, "Not Applicable")</f>
         <v>1</v>
       </c>
     </row>
@@ -5334,7 +5495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -5373,29 +5534,29 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <f>COUNTIF(Sheet1!Q$2:Q$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!Q$2:Q$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f>COUNTIF(Sheet1!R$2:R$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!R$2:R$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f>COUNTIF(Sheet1!S$2:S$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!S$2:S$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="G4" t="s">
         <v>117</v>
       </c>
       <c r="H4">
-        <f>COUNTIF(Sheet1!AP$2:$AP17, 1)</f>
+        <f>COUNTIF('Raw Data'!AP$2:$AP17, 1)</f>
         <v>1</v>
       </c>
       <c r="I4" t="s">
         <v>113</v>
       </c>
       <c r="J4">
-        <f>COUNTIF(Sheet1!AQ$2:AQ$17, 1)</f>
+        <f>COUNTIF('Raw Data'!AQ$2:AQ$17, 1)</f>
         <v>5</v>
       </c>
     </row>
@@ -5404,29 +5565,29 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <f>COUNTIF(Sheet1!Q$2:Q$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!Q$2:Q$17, "Disagree")</f>
         <v>0</v>
       </c>
       <c r="D5">
-        <f>COUNTIF(Sheet1!R$2:R$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!R$2:R$17, "Disagree")</f>
         <v>0</v>
       </c>
       <c r="E5">
-        <f>COUNTIF(Sheet1!S$2:S$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!S$2:S$17, "Disagree")</f>
         <v>0</v>
       </c>
       <c r="G5" t="s">
         <v>118</v>
       </c>
       <c r="H5">
-        <f>COUNTIF(Sheet1!AP$2:$AP18, 2)</f>
+        <f>COUNTIF('Raw Data'!AP$2:$AP18, 2)</f>
         <v>4</v>
       </c>
       <c r="I5" t="s">
         <v>115</v>
       </c>
       <c r="J5">
-        <f>COUNTIF(Sheet1!AQ$2:AQ$17, 2)</f>
+        <f>COUNTIF('Raw Data'!AQ$2:AQ$17, 2)</f>
         <v>2</v>
       </c>
     </row>
@@ -5435,29 +5596,29 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <f>COUNTIF(Sheet1!Q$2:Q$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!Q$2:Q$17, "Neutral")</f>
         <v>2</v>
       </c>
       <c r="D6">
-        <f>COUNTIF(Sheet1!R$2:R$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!R$2:R$17, "Neutral")</f>
         <v>3</v>
       </c>
       <c r="E6">
-        <f>COUNTIF(Sheet1!S$2:S$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!S$2:S$17, "Neutral")</f>
         <v>4</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
       </c>
       <c r="H6">
-        <f>COUNTIF(Sheet1!AP$2:$AP19, 3)</f>
+        <f>COUNTIF('Raw Data'!AP$2:$AP19, 3)</f>
         <v>3</v>
       </c>
       <c r="I6" t="s">
         <v>116</v>
       </c>
       <c r="J6">
-        <f>COUNTIF(Sheet1!AQ$2:AQ$17, 3)</f>
+        <f>COUNTIF('Raw Data'!AQ$2:AQ$17, 3)</f>
         <v>7</v>
       </c>
     </row>
@@ -5466,29 +5627,29 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <f>COUNTIF(Sheet1!Q$2:Q$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!Q$2:Q$17, "Agree")</f>
         <v>5</v>
       </c>
       <c r="D7">
-        <f>COUNTIF(Sheet1!R$2:R$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!R$2:R$17, "Agree")</f>
         <v>2</v>
       </c>
       <c r="E7">
-        <f>COUNTIF(Sheet1!S$2:S$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!S$2:S$17, "Agree")</f>
         <v>2</v>
       </c>
       <c r="G7" t="s">
         <v>119</v>
       </c>
       <c r="H7">
-        <f>COUNTIF(Sheet1!AP$2:$AP20, 4)</f>
+        <f>COUNTIF('Raw Data'!AP$2:$AP20, 4)</f>
         <v>5</v>
       </c>
       <c r="I7" t="s">
         <v>114</v>
       </c>
       <c r="J7">
-        <f>COUNTIF(Sheet1!AQ$2:AQ$17, 4)</f>
+        <f>COUNTIF('Raw Data'!AQ$2:AQ$17, 4)</f>
         <v>1</v>
       </c>
     </row>
@@ -5497,22 +5658,22 @@
         <v>15</v>
       </c>
       <c r="C8">
-        <f>COUNTIF(Sheet1!Q$2:Q$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!Q$2:Q$17, "Strongly agree")</f>
         <v>8</v>
       </c>
       <c r="D8">
-        <f>COUNTIF(Sheet1!R$2:R$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!R$2:R$17, "Strongly agree")</f>
         <v>10</v>
       </c>
       <c r="E8">
-        <f>COUNTIF(Sheet1!S$2:S$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!S$2:S$17, "Strongly agree")</f>
         <v>8</v>
       </c>
       <c r="G8" t="s">
         <v>120</v>
       </c>
       <c r="H8">
-        <f>COUNTIF(Sheet1!AP$2:$AP21, 5)</f>
+        <f>COUNTIF('Raw Data'!AP$2:$AP21, 5)</f>
         <v>2</v>
       </c>
     </row>
@@ -5521,15 +5682,15 @@
         <v>112</v>
       </c>
       <c r="C9">
-        <f>COUNTIF(Sheet1!Q$2:Q$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!Q$2:Q$17, "Not Applicable")</f>
         <v>0</v>
       </c>
       <c r="D9">
-        <f>COUNTIF(Sheet1!R$2:R$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!R$2:R$17, "Not Applicable")</f>
         <v>0</v>
       </c>
       <c r="E9">
-        <f>COUNTIF(Sheet1!S$2:S$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!S$2:S$17, "Not Applicable")</f>
         <v>1</v>
       </c>
     </row>
@@ -5604,19 +5765,19 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:15">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:15">
       <c r="B5" t="s">
@@ -5658,31 +5819,31 @@
         <v>125</v>
       </c>
       <c r="B6">
-        <f>COUNTIF(Sheet1!U$2:U$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!U$2:U$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="C6">
-        <f>COUNTIF(Sheet1!U$2:U$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!U$2:U$17, "Disagree")</f>
         <v>0</v>
       </c>
       <c r="D6">
-        <f>COUNTIF(Sheet1!U$2:U$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!U$2:U$17, "Neutral")</f>
         <v>0</v>
       </c>
       <c r="E6">
-        <f>COUNTIF(Sheet1!U$2:U$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!U$2:U$17, "Agree")</f>
         <v>8</v>
       </c>
       <c r="F6">
-        <f>COUNTIF(Sheet1!U$2:U$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!U$2:U$17, "Strongly agree")</f>
         <v>7</v>
       </c>
       <c r="G6">
-        <f>COUNTIF(Sheet1!U$2:U$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!U$2:U$17, "Not Applicable")</f>
         <v>0</v>
       </c>
       <c r="I6">
-        <f>SUM(B6:G6)</f>
+        <f t="shared" ref="I6:I13" si="0">SUM(B6:G6)</f>
         <v>15</v>
       </c>
       <c r="K6">
@@ -5707,43 +5868,43 @@
         <v>126</v>
       </c>
       <c r="B7">
-        <f>COUNTIF(Sheet1!V$2:V$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!V$2:V$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="C7">
-        <f>COUNTIF(Sheet1!V$2:V$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!V$2:V$17, "Disagree")</f>
         <v>0</v>
       </c>
       <c r="D7">
-        <f>COUNTIF(Sheet1!V$2:V$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!V$2:V$17, "Neutral")</f>
         <v>0</v>
       </c>
       <c r="E7">
-        <f>COUNTIF(Sheet1!V$2:V$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!V$2:V$17, "Agree")</f>
         <v>2</v>
       </c>
       <c r="F7">
-        <f>COUNTIF(Sheet1!V$2:V$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!V$2:V$17, "Strongly agree")</f>
         <v>13</v>
       </c>
       <c r="G7">
-        <f>COUNTIF(Sheet1!V$2:V$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!V$2:V$17, "Not Applicable")</f>
         <v>0</v>
       </c>
       <c r="I7">
-        <f>SUM(B7:G7)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="K7">
-        <f t="shared" ref="K7:K13" si="0">B7*1 +C7*2 +D7*3 + E7*4 + F7*5</f>
+        <f t="shared" ref="K7:K13" si="1">B7*1 +C7*2 +D7*3 + E7*4 + F7*5</f>
         <v>73</v>
       </c>
       <c r="L7">
-        <f t="shared" ref="L7:L13" si="1">SUM(B7:F7)</f>
+        <f t="shared" ref="L7:L13" si="2">SUM(B7:F7)</f>
         <v>15</v>
       </c>
       <c r="M7">
-        <f t="shared" ref="M7:M13" si="2">K7/L7</f>
+        <f t="shared" ref="M7:M13" si="3">K7/L7</f>
         <v>4.8666666666666663</v>
       </c>
     </row>
@@ -5752,43 +5913,43 @@
         <v>127</v>
       </c>
       <c r="B8">
-        <f>COUNTIF(Sheet1!W$2:W$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!W$2:W$17, "Strongly disagree")</f>
         <v>1</v>
       </c>
       <c r="C8">
-        <f>COUNTIF(Sheet1!W$2:W$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!W$2:W$17, "Disagree")</f>
         <v>1</v>
       </c>
       <c r="D8">
-        <f>COUNTIF(Sheet1!W$2:W$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!W$2:W$17, "Neutral")</f>
         <v>2</v>
       </c>
       <c r="E8">
-        <f>COUNTIF(Sheet1!W$2:W$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!W$2:W$17, "Agree")</f>
         <v>3</v>
       </c>
       <c r="F8">
-        <f>COUNTIF(Sheet1!W$2:W$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!W$2:W$17, "Strongly agree")</f>
         <v>4</v>
       </c>
       <c r="G8">
-        <f>COUNTIF(Sheet1!W$2:W$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!W$2:W$17, "Not Applicable")</f>
         <v>4</v>
       </c>
       <c r="I8">
-        <f>SUM(B8:G8)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="L8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="M8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.7272727272727271</v>
       </c>
     </row>
@@ -5797,43 +5958,43 @@
         <v>128</v>
       </c>
       <c r="B9">
-        <f>COUNTIF(Sheet1!X$2:X$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!X$2:X$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="C9">
-        <f>COUNTIF(Sheet1!X$2:X$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!X$2:X$17, "Disagree")</f>
         <v>1</v>
       </c>
       <c r="D9">
-        <f>COUNTIF(Sheet1!X$2:X$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!X$2:X$17, "Neutral")</f>
         <v>3</v>
       </c>
       <c r="E9">
-        <f>COUNTIF(Sheet1!X$2:X$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!X$2:X$17, "Agree")</f>
         <v>3</v>
       </c>
       <c r="F9">
-        <f>COUNTIF(Sheet1!X$2:X$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!X$2:X$17, "Strongly agree")</f>
         <v>6</v>
       </c>
       <c r="G9">
-        <f>COUNTIF(Sheet1!X$2:X$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!X$2:X$17, "Not Applicable")</f>
         <v>2</v>
       </c>
       <c r="I9">
-        <f>SUM(B9:G9)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="K9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="L9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="M9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.0769230769230766</v>
       </c>
     </row>
@@ -5842,43 +6003,43 @@
         <v>129</v>
       </c>
       <c r="B10">
-        <f>COUNTIF(Sheet1!Y$2:Y$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!Y$2:Y$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="C10">
-        <f>COUNTIF(Sheet1!Y$2:Y$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!Y$2:Y$17, "Disagree")</f>
         <v>2</v>
       </c>
       <c r="D10">
-        <f>COUNTIF(Sheet1!Y$2:Y$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!Y$2:Y$17, "Neutral")</f>
         <v>2</v>
       </c>
       <c r="E10">
-        <f>COUNTIF(Sheet1!Y$2:Y$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!Y$2:Y$17, "Agree")</f>
         <v>4</v>
       </c>
       <c r="F10">
-        <f>COUNTIF(Sheet1!Y$2:Y$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!Y$2:Y$17, "Strongly agree")</f>
         <v>5</v>
       </c>
       <c r="G10">
-        <f>COUNTIF(Sheet1!Y$2:Y$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!Y$2:Y$17, "Not Applicable")</f>
         <v>2</v>
       </c>
       <c r="I10">
-        <f>SUM(B10:G10)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="K10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="L10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="M10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.9230769230769229</v>
       </c>
     </row>
@@ -5887,43 +6048,43 @@
         <v>130</v>
       </c>
       <c r="B11">
-        <f>COUNTIF(Sheet1!Z$2:Z$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!Z$2:Z$17, "Strongly disagree")</f>
         <v>1</v>
       </c>
       <c r="C11">
-        <f>COUNTIF(Sheet1!Z$2:Z$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!Z$2:Z$17, "Disagree")</f>
         <v>1</v>
       </c>
       <c r="D11">
-        <f>COUNTIF(Sheet1!Z$2:Z$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!Z$2:Z$17, "Neutral")</f>
         <v>0</v>
       </c>
       <c r="E11">
-        <f>COUNTIF(Sheet1!Z$2:Z$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!Z$2:Z$17, "Agree")</f>
         <v>3</v>
       </c>
       <c r="F11">
-        <f>COUNTIF(Sheet1!Z$2:Z$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!Z$2:Z$17, "Strongly agree")</f>
         <v>10</v>
       </c>
       <c r="G11">
-        <f>COUNTIF(Sheet1!Z$2:Z$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!Z$2:Z$17, "Not Applicable")</f>
         <v>0</v>
       </c>
       <c r="I11">
-        <f>SUM(B11:G11)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="K11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
       <c r="L11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.333333333333333</v>
       </c>
     </row>
@@ -5932,43 +6093,43 @@
         <v>132</v>
       </c>
       <c r="B12">
-        <f>COUNTIF(Sheet1!AA$2:AA$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!AA$2:AA$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="C12">
-        <f>COUNTIF(Sheet1!AA$2:AA$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!AA$2:AA$17, "Disagree")</f>
         <v>0</v>
       </c>
       <c r="D12">
-        <f>COUNTIF(Sheet1!AA$2:AA$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!AA$2:AA$17, "Neutral")</f>
         <v>2</v>
       </c>
       <c r="E12">
-        <f>COUNTIF(Sheet1!AA$2:AA$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!AA$2:AA$17, "Agree")</f>
         <v>0</v>
       </c>
       <c r="F12">
-        <f>COUNTIF(Sheet1!AA$2:AA$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!AA$2:AA$17, "Strongly agree")</f>
         <v>13</v>
       </c>
       <c r="G12">
-        <f>COUNTIF(Sheet1!AA$2:AA$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!AA$2:AA$17, "Not Applicable")</f>
         <v>0</v>
       </c>
       <c r="I12">
-        <f>SUM(B12:G12)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="K12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="L12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.7333333333333334</v>
       </c>
     </row>
@@ -5977,60 +6138,60 @@
         <v>133</v>
       </c>
       <c r="B13">
-        <f>COUNTIF(Sheet1!AB$2:AB$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!AB$2:AB$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="C13">
-        <f>COUNTIF(Sheet1!AB$2:AB$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!AB$2:AB$17, "Disagree")</f>
         <v>1</v>
       </c>
       <c r="D13">
-        <f>COUNTIF(Sheet1!AB$2:AB$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!AB$2:AB$17, "Neutral")</f>
         <v>2</v>
       </c>
       <c r="E13">
-        <f>COUNTIF(Sheet1!AB$2:AB$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!AB$2:AB$17, "Agree")</f>
         <v>3</v>
       </c>
       <c r="F13">
-        <f>COUNTIF(Sheet1!AB$2:AB$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!AB$2:AB$17, "Strongly agree")</f>
         <v>5</v>
       </c>
       <c r="G13">
-        <f>COUNTIF(Sheet1!AB$2:AB$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!AB$2:AB$17, "Not Applicable")</f>
         <v>4</v>
       </c>
       <c r="I13">
-        <f>SUM(B13:G13)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="K13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="L13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="M13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.0909090909090908</v>
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:15">
       <c r="B16" t="s">
@@ -6072,31 +6233,31 @@
         <v>134</v>
       </c>
       <c r="B17">
-        <f>COUNTIF(Sheet1!AC$2:AC$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!AC$2:AC$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="C17">
-        <f>COUNTIF(Sheet1!AC$2:AC$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!AC$2:AC$17, "Disagree")</f>
         <v>2</v>
       </c>
       <c r="D17">
-        <f>COUNTIF(Sheet1!AC$2:AC$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!AC$2:AC$17, "Neutral")</f>
         <v>1</v>
       </c>
       <c r="E17">
-        <f>COUNTIF(Sheet1!AC$2:AC$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!AC$2:AC$17, "Agree")</f>
         <v>4</v>
       </c>
       <c r="F17">
-        <f>COUNTIF(Sheet1!AC$2:AC$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!AC$2:AC$17, "Strongly agree")</f>
         <v>2</v>
       </c>
       <c r="G17">
-        <f>COUNTIF(Sheet1!AC$2:AC$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!AC$2:AC$17, "Not Applicable")</f>
         <v>6</v>
       </c>
       <c r="I17">
-        <f>SUM(B17:G17)</f>
+        <f t="shared" ref="I17:I23" si="4">SUM(B17:G17)</f>
         <v>15</v>
       </c>
       <c r="K17">
@@ -6121,43 +6282,43 @@
         <v>136</v>
       </c>
       <c r="B18">
-        <f>COUNTIF(Sheet1!AD$2:AD$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!AD$2:AD$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="C18">
-        <f>COUNTIF(Sheet1!AD$2:AD$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!AD$2:AD$17, "Disagree")</f>
         <v>0</v>
       </c>
       <c r="D18">
-        <f>COUNTIF(Sheet1!AD$2:AD$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!AD$2:AD$17, "Neutral")</f>
         <v>5</v>
       </c>
       <c r="E18">
-        <f>COUNTIF(Sheet1!AD$2:AD$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!AD$2:AD$17, "Agree")</f>
         <v>1</v>
       </c>
       <c r="F18">
-        <f>COUNTIF(Sheet1!AD$2:AD$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!AD$2:AD$17, "Strongly agree")</f>
         <v>3</v>
       </c>
       <c r="G18">
-        <f>COUNTIF(Sheet1!AD$2:AD$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!AD$2:AD$17, "Not Applicable")</f>
         <v>6</v>
       </c>
       <c r="I18">
-        <f>SUM(B18:G18)</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="K18">
-        <f t="shared" ref="K18:K24" si="3">B18*1 +C18*2 +D18*3 + E18*4 + F18*5</f>
+        <f t="shared" ref="K18:K23" si="5">B18*1 +C18*2 +D18*3 + E18*4 + F18*5</f>
         <v>34</v>
       </c>
       <c r="L18">
-        <f t="shared" ref="L18:L24" si="4">SUM(B18:F18)</f>
+        <f t="shared" ref="L18:L23" si="6">SUM(B18:F18)</f>
         <v>9</v>
       </c>
       <c r="M18">
-        <f t="shared" ref="M18:M24" si="5">K18/L18</f>
+        <f t="shared" ref="M18:M23" si="7">K18/L18</f>
         <v>3.7777777777777777</v>
       </c>
     </row>
@@ -6166,43 +6327,43 @@
         <v>137</v>
       </c>
       <c r="B19">
-        <f>COUNTIF(Sheet1!AE$2:AE$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!AE$2:AE$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="C19">
-        <f>COUNTIF(Sheet1!AE$2:AE$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!AE$2:AE$17, "Disagree")</f>
         <v>0</v>
       </c>
       <c r="D19">
-        <f>COUNTIF(Sheet1!AE$2:AE$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!AE$2:AE$17, "Neutral")</f>
         <v>3</v>
       </c>
       <c r="E19">
-        <f>COUNTIF(Sheet1!AE$2:AE$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!AE$2:AE$17, "Agree")</f>
         <v>4</v>
       </c>
       <c r="F19">
-        <f>COUNTIF(Sheet1!AE$2:AE$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!AE$2:AE$17, "Strongly agree")</f>
         <v>5</v>
       </c>
       <c r="G19">
-        <f>COUNTIF(Sheet1!AE$2:AE$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!AE$2:AE$17, "Not Applicable")</f>
         <v>3</v>
       </c>
       <c r="I19">
-        <f>SUM(B19:G19)</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="K19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
       <c r="L19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="M19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.166666666666667</v>
       </c>
     </row>
@@ -6211,43 +6372,43 @@
         <v>138</v>
       </c>
       <c r="B20">
-        <f>COUNTIF(Sheet1!AF$2:AF$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!AF$2:AF$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="C20">
-        <f>COUNTIF(Sheet1!AF$2:AF$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!AF$2:AF$17, "Disagree")</f>
         <v>1</v>
       </c>
       <c r="D20">
-        <f>COUNTIF(Sheet1!AF$2:AF$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!AF$2:AF$17, "Neutral")</f>
         <v>2</v>
       </c>
       <c r="E20">
-        <f>COUNTIF(Sheet1!AF$2:AF$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!AF$2:AF$17, "Agree")</f>
         <v>3</v>
       </c>
       <c r="F20">
-        <f>COUNTIF(Sheet1!AF$2:AF$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!AF$2:AF$17, "Strongly agree")</f>
         <v>6</v>
       </c>
       <c r="G20">
-        <f>COUNTIF(Sheet1!AF$2:AF$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!AF$2:AF$17, "Not Applicable")</f>
         <v>3</v>
       </c>
       <c r="I20">
-        <f>SUM(B20:G20)</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="K20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
       <c r="L20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="M20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.166666666666667</v>
       </c>
     </row>
@@ -6256,43 +6417,43 @@
         <v>139</v>
       </c>
       <c r="B21">
-        <f>COUNTIF(Sheet1!AG$2:AG$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!AG$2:AG$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="C21">
-        <f>COUNTIF(Sheet1!AG$2:AG$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!AG$2:AG$17, "Disagree")</f>
         <v>1</v>
       </c>
       <c r="D21">
-        <f>COUNTIF(Sheet1!AG$2:AG$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!AG$2:AG$17, "Neutral")</f>
         <v>2</v>
       </c>
       <c r="E21">
-        <f>COUNTIF(Sheet1!AG$2:AG$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!AG$2:AG$17, "Agree")</f>
         <v>5</v>
       </c>
       <c r="F21">
-        <f>COUNTIF(Sheet1!AG$2:AG$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!AG$2:AG$17, "Strongly agree")</f>
         <v>6</v>
       </c>
       <c r="G21">
-        <f>COUNTIF(Sheet1!AG$2:AG$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!AG$2:AG$17, "Not Applicable")</f>
         <v>1</v>
       </c>
       <c r="I21">
-        <f>SUM(B21:G21)</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="K21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>58</v>
       </c>
       <c r="L21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="M21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.1428571428571432</v>
       </c>
     </row>
@@ -6301,43 +6462,43 @@
         <v>140</v>
       </c>
       <c r="B22">
-        <f>COUNTIF(Sheet1!AH$2:AH$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!AH$2:AH$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="C22">
-        <f>COUNTIF(Sheet1!AH$2:AH$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!AH$2:AH$17, "Disagree")</f>
         <v>1</v>
       </c>
       <c r="D22">
-        <f>COUNTIF(Sheet1!AH$2:AH$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!AH$2:AH$17, "Neutral")</f>
         <v>4</v>
       </c>
       <c r="E22">
-        <f>COUNTIF(Sheet1!AH$2:AH$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!AH$2:AH$17, "Agree")</f>
         <v>2</v>
       </c>
       <c r="F22">
-        <f>COUNTIF(Sheet1!AH$2:AH$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!AH$2:AH$17, "Strongly agree")</f>
         <v>7</v>
       </c>
       <c r="G22">
-        <f>COUNTIF(Sheet1!AH$2:AH$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!AH$2:AH$17, "Not Applicable")</f>
         <v>1</v>
       </c>
       <c r="I22">
-        <f>SUM(B22:G22)</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="K22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>57</v>
       </c>
       <c r="L22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="M22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.0714285714285712</v>
       </c>
     </row>
@@ -6346,60 +6507,60 @@
         <v>141</v>
       </c>
       <c r="B23">
-        <f>COUNTIF(Sheet1!AI$2:AI$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!AI$2:AI$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="C23">
-        <f>COUNTIF(Sheet1!AI$2:AI$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!AI$2:AI$17, "Disagree")</f>
         <v>0</v>
       </c>
       <c r="D23">
-        <f>COUNTIF(Sheet1!AI$2:AI$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!AI$2:AI$17, "Neutral")</f>
         <v>3</v>
       </c>
       <c r="E23">
-        <f>COUNTIF(Sheet1!AI$2:AI$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!AI$2:AI$17, "Agree")</f>
         <v>8</v>
       </c>
       <c r="F23">
-        <f>COUNTIF(Sheet1!AI$2:AI$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!AI$2:AI$17, "Strongly agree")</f>
         <v>4</v>
       </c>
       <c r="G23">
-        <f>COUNTIF(Sheet1!AI$2:AI$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!AI$2:AI$17, "Not Applicable")</f>
         <v>0</v>
       </c>
       <c r="I23">
-        <f>SUM(B23:G23)</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="K23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>61</v>
       </c>
       <c r="L23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="M23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.0666666666666664</v>
       </c>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:15">
       <c r="B27" t="s">
@@ -6441,27 +6602,27 @@
         <v>144</v>
       </c>
       <c r="B28">
-        <f>COUNTIF(Sheet1!AJ$2:AJ$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!AJ$2:AJ$17, "Strongly disagree")</f>
         <v>1</v>
       </c>
       <c r="C28">
-        <f>COUNTIF(Sheet1!AJ$2:AJ$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!AJ$2:AJ$17, "Disagree")</f>
         <v>1</v>
       </c>
       <c r="D28">
-        <f>COUNTIF(Sheet1!AJ$2:AJ$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!AJ$2:AJ$17, "Neutral")</f>
         <v>1</v>
       </c>
       <c r="E28">
-        <f>COUNTIF(Sheet1!AJ$2:AJ$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!AJ$2:AJ$17, "Agree")</f>
         <v>7</v>
       </c>
       <c r="F28">
-        <f>COUNTIF(Sheet1!AJ$2:AJ$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!AJ$2:AJ$17, "Strongly agree")</f>
         <v>5</v>
       </c>
       <c r="G28">
-        <f>COUNTIF(Sheet1!AJ$2:AJ$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!AJ$2:AJ$17, "Not Applicable")</f>
         <v>0</v>
       </c>
       <c r="I28">
@@ -6490,27 +6651,27 @@
         <v>145</v>
       </c>
       <c r="B29">
-        <f>COUNTIF(Sheet1!AK$2:AK$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!AK$2:AK$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="C29">
-        <f>COUNTIF(Sheet1!AK$2:AK$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!AK$2:AK$17, "Disagree")</f>
         <v>2</v>
       </c>
       <c r="D29">
-        <f>COUNTIF(Sheet1!AK$2:AK$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!AK$2:AK$17, "Neutral")</f>
         <v>1</v>
       </c>
       <c r="E29">
-        <f>COUNTIF(Sheet1!AK$2:AK$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!AK$2:AK$17, "Agree")</f>
         <v>8</v>
       </c>
       <c r="F29">
-        <f>COUNTIF(Sheet1!AK$2:AK$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!AK$2:AK$17, "Strongly agree")</f>
         <v>4</v>
       </c>
       <c r="G29">
-        <f>COUNTIF(Sheet1!AK$2:AK$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!AK$2:AK$17, "Not Applicable")</f>
         <v>0</v>
       </c>
       <c r="I29">
@@ -6518,15 +6679,15 @@
         <v>15</v>
       </c>
       <c r="K29">
-        <f t="shared" ref="K29:K34" si="6">B29*1 +C29*2 +D29*3 + E29*4 + F29*5</f>
+        <f t="shared" ref="K29:K31" si="8">B29*1 +C29*2 +D29*3 + E29*4 + F29*5</f>
         <v>59</v>
       </c>
       <c r="L29">
-        <f t="shared" ref="L29:L34" si="7">SUM(B29:F29)</f>
+        <f t="shared" ref="L29:L31" si="9">SUM(B29:F29)</f>
         <v>15</v>
       </c>
       <c r="M29">
-        <f t="shared" ref="M29:M34" si="8">K29/L29</f>
+        <f t="shared" ref="M29:M31" si="10">K29/L29</f>
         <v>3.9333333333333331</v>
       </c>
     </row>
@@ -6535,27 +6696,27 @@
         <v>146</v>
       </c>
       <c r="B30">
-        <f>COUNTIF(Sheet1!AL$2:AL$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!AL$2:AL$17, "Strongly disagree")</f>
         <v>1</v>
       </c>
       <c r="C30">
-        <f>COUNTIF(Sheet1!AL$2:AL$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!AL$2:AL$17, "Disagree")</f>
         <v>2</v>
       </c>
       <c r="D30">
-        <f>COUNTIF(Sheet1!AL$2:AL$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!AL$2:AL$17, "Neutral")</f>
         <v>1</v>
       </c>
       <c r="E30">
-        <f>COUNTIF(Sheet1!AL$2:AL$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!AL$2:AL$17, "Agree")</f>
         <v>4</v>
       </c>
       <c r="F30">
-        <f>COUNTIF(Sheet1!AL$2:AL$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!AL$2:AL$17, "Strongly agree")</f>
         <v>4</v>
       </c>
       <c r="G30">
-        <f>COUNTIF(Sheet1!AL$2:AL$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!AL$2:AL$17, "Not Applicable")</f>
         <v>3</v>
       </c>
       <c r="I30">
@@ -6563,15 +6724,15 @@
         <v>15</v>
       </c>
       <c r="K30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>44</v>
       </c>
       <c r="L30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="M30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.6666666666666665</v>
       </c>
     </row>
@@ -6580,27 +6741,27 @@
         <v>147</v>
       </c>
       <c r="B31">
-        <f>COUNTIF(Sheet1!AM$2:AM$17, "Strongly disagree")</f>
+        <f>COUNTIF('Raw Data'!AM$2:AM$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
       <c r="C31">
-        <f>COUNTIF(Sheet1!AM$2:AM$17, "Disagree")</f>
+        <f>COUNTIF('Raw Data'!AM$2:AM$17, "Disagree")</f>
         <v>0</v>
       </c>
       <c r="D31">
-        <f>COUNTIF(Sheet1!AM$2:AM$17, "Neutral")</f>
+        <f>COUNTIF('Raw Data'!AM$2:AM$17, "Neutral")</f>
         <v>2</v>
       </c>
       <c r="E31">
-        <f>COUNTIF(Sheet1!AM$2:AM$17, "Agree")</f>
+        <f>COUNTIF('Raw Data'!AM$2:AM$17, "Agree")</f>
         <v>7</v>
       </c>
       <c r="F31">
-        <f>COUNTIF(Sheet1!AM$2:AM$17, "Strongly agree")</f>
+        <f>COUNTIF('Raw Data'!AM$2:AM$17, "Strongly agree")</f>
         <v>6</v>
       </c>
       <c r="G31">
-        <f>COUNTIF(Sheet1!AM$2:AM$17, "Not Applicable")</f>
+        <f>COUNTIF('Raw Data'!AM$2:AM$17, "Not Applicable")</f>
         <v>0</v>
       </c>
       <c r="I31">
@@ -6608,15 +6769,15 @@
         <v>15</v>
       </c>
       <c r="K31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>64</v>
       </c>
       <c r="L31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="M31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.2666666666666666</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated evaluation price performance
</commit_message>
<xml_diff>
--- a/documents/resources/evaluation/usability/Survey-Compiled.xlsx
+++ b/documents/resources/evaluation/usability/Survey-Compiled.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="540" windowWidth="24880" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="2640" yWindow="540" windowWidth="24880" windowHeight="16740" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="176">
   <si>
     <t>Male</t>
   </si>
@@ -403,9 +403,6 @@
     <t>Is command line a barrier to reproduce a simulation</t>
   </si>
   <si>
-    <t>how easy it is to use this system</t>
-  </si>
-  <si>
     <t>It was simple to use this system</t>
   </si>
   <si>
@@ -499,9 +496,6 @@
     <t>SUM</t>
   </si>
   <si>
-    <t>SCORE</t>
-  </si>
-  <si>
     <t>TAKEN OUT BECAUSE RESPONDENT SKIP BOTH SCENARIO</t>
   </si>
   <si>
@@ -548,6 +542,18 @@
   </si>
   <si>
     <t>TOTAL ASQ SCORE</t>
+  </si>
+  <si>
+    <t>ASQ SCORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overall, I am satisfied with how easy it is to use this system </t>
+  </si>
+  <si>
+    <t>OVERALL USABILITY FINAL SCORE</t>
+  </si>
+  <si>
+    <t>Overall Usability</t>
   </si>
 </sst>
 </file>
@@ -623,8 +629,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="141">
+  <cellStyleXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -783,7 +803,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="141">
+  <cellStyles count="155">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -854,6 +874,13 @@
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -924,6 +951,13 @@
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3562,8 +3596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AN2" sqref="AN2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5682,7 +5716,7 @@
     </row>
     <row r="22" spans="1:43">
       <c r="A22" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -5728,7 +5762,7 @@
         <v>4</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="N23" s="7">
         <v>1</v>
@@ -5749,7 +5783,7 @@
         <v>4</v>
       </c>
       <c r="T23" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="U23" s="7" t="s">
         <v>4</v>
@@ -5809,10 +5843,10 @@
         <v>4</v>
       </c>
       <c r="AN23" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AO23" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AP23" s="7">
         <v>1</v>
@@ -5839,7 +5873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L56"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="M49" sqref="M49"/>
     </sheetView>
   </sheetViews>
@@ -5854,7 +5888,7 @@
         <v>68</v>
       </c>
       <c r="L2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="2:12">
@@ -5866,7 +5900,7 @@
         <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L3">
         <f>COUNTIF('Raw Data'!F$2:F$17, 1)</f>
@@ -5882,7 +5916,7 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L4">
         <f>COUNTIF('Raw Data'!F$2:F$17, 2)</f>
@@ -5891,7 +5925,7 @@
     </row>
     <row r="5" spans="2:12">
       <c r="K5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="L5">
         <f>COUNTIF('Raw Data'!F$2:F$17, 3)</f>
@@ -5900,7 +5934,7 @@
     </row>
     <row r="6" spans="2:12">
       <c r="K6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L6">
         <f>COUNTIF('Raw Data'!F$2:F$17, 4)</f>
@@ -5909,7 +5943,7 @@
     </row>
     <row r="7" spans="2:12">
       <c r="K7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L7">
         <f>COUNTIF('Raw Data'!F$2:F$17, 5)</f>
@@ -5924,12 +5958,12 @@
     </row>
     <row r="11" spans="2:12">
       <c r="L11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="2:12">
       <c r="K12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L12">
         <f>COUNTIF('Raw Data'!G$2:G$17, 1)</f>
@@ -5938,7 +5972,7 @@
     </row>
     <row r="13" spans="2:12">
       <c r="K13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L13">
         <f>COUNTIF('Raw Data'!G$2:G$17, 2)</f>
@@ -5947,7 +5981,7 @@
     </row>
     <row r="14" spans="2:12">
       <c r="K14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="L14">
         <f>COUNTIF('Raw Data'!G$2:G$17, 3)</f>
@@ -5956,7 +5990,7 @@
     </row>
     <row r="15" spans="2:12">
       <c r="K15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L15">
         <f>COUNTIF('Raw Data'!G$2:G$17, 4)</f>
@@ -5965,7 +5999,7 @@
     </row>
     <row r="16" spans="2:12">
       <c r="K16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L16">
         <f>COUNTIF('Raw Data'!G$2:G$17, 5)</f>
@@ -5980,12 +6014,12 @@
     </row>
     <row r="19" spans="2:12">
       <c r="L19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="2:12">
       <c r="K20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L20">
         <f>COUNTIF('Raw Data'!H$2:H$17, 1)</f>
@@ -5997,7 +6031,7 @@
         <v>107</v>
       </c>
       <c r="K21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L21">
         <f>COUNTIF('Raw Data'!H$2:H$17, 2)</f>
@@ -6013,7 +6047,7 @@
         <v>7</v>
       </c>
       <c r="K22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="L22">
         <f>COUNTIF('Raw Data'!H$2:H$17, 3)</f>
@@ -6029,7 +6063,7 @@
         <v>2</v>
       </c>
       <c r="K23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L23">
         <f>COUNTIF('Raw Data'!H$2:H$17, 4)</f>
@@ -6045,7 +6079,7 @@
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L24">
         <f>COUNTIF('Raw Data'!H$2:H$17, 5)</f>
@@ -6099,7 +6133,7 @@
     </row>
     <row r="40" spans="2:3">
       <c r="C40" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="16">
@@ -6122,7 +6156,7 @@
     </row>
     <row r="43" spans="2:3" ht="16">
       <c r="B43" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C43">
         <f>COUNTIF('Raw Data'!$E$2:$E$17, "physics/Biophysics")</f>
@@ -6197,7 +6231,7 @@
   <dimension ref="B3:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="B12" sqref="B12:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6214,13 +6248,13 @@
   <sheetData>
     <row r="3" spans="2:10">
       <c r="C3" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>111</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F3" s="3"/>
       <c r="H3" s="3" t="s">
@@ -6397,7 +6431,7 @@
     </row>
     <row r="11" spans="2:10">
       <c r="B11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C11">
         <f>SUM(C4:C9)</f>
@@ -6422,7 +6456,7 @@
     </row>
     <row r="12" spans="2:10">
       <c r="B12" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="C12">
         <f>(C4*1 +C5*2 +C6* 3 +C7*4 +C8 * 5) /SUM(C4:C8)</f>
@@ -6439,7 +6473,7 @@
     </row>
     <row r="14" spans="2:10">
       <c r="B14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C14">
         <f>AVERAGE(C12:E12)</f>
@@ -6460,10 +6494,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J12"/>
+  <dimension ref="B3:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6480,13 +6514,13 @@
   <sheetData>
     <row r="3" spans="2:10">
       <c r="C3" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>111</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F3" s="3"/>
       <c r="H3" s="3" t="s">
@@ -6663,7 +6697,7 @@
     </row>
     <row r="11" spans="2:10">
       <c r="B11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C11">
         <f>SUM(C4:C9)</f>
@@ -6688,7 +6722,7 @@
     </row>
     <row r="12" spans="2:10">
       <c r="B12" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="C12">
         <f>(C4*1 +C5*2 +C6* 3 +C7*4 +C8 * 5) /SUM(C4:C8)</f>
@@ -6701,6 +6735,15 @@
       <c r="E12">
         <f t="shared" si="2"/>
         <v>4.2857142857142856</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" t="s">
+        <v>171</v>
+      </c>
+      <c r="C14">
+        <f>AVERAGE(C12:E12)</f>
+        <v>4.3841269841269837</v>
       </c>
     </row>
   </sheetData>
@@ -6717,10 +6760,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:O31"/>
+  <dimension ref="A4:O37"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6733,7 +6776,7 @@
   <sheetData>
     <row r="4" spans="1:15">
       <c r="A4" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -6766,24 +6809,24 @@
         <v>112</v>
       </c>
       <c r="I5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K5" t="s">
+        <v>147</v>
+      </c>
+      <c r="L5" t="s">
         <v>148</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>149</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>150</v>
-      </c>
-      <c r="O5" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>173</v>
       </c>
       <c r="B6">
         <f>COUNTIF('Raw Data'!U$2:U$17, "Strongly disagree")</f>
@@ -6832,7 +6875,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B7">
         <f>COUNTIF('Raw Data'!V$2:V$17, "Strongly disagree")</f>
@@ -6877,7 +6920,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B8">
         <f>COUNTIF('Raw Data'!W$2:W$17, "Strongly disagree")</f>
@@ -6922,7 +6965,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B9">
         <f>COUNTIF('Raw Data'!X$2:X$17, "Strongly disagree")</f>
@@ -6967,7 +7010,7 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B10">
         <f>COUNTIF('Raw Data'!Y$2:Y$17, "Strongly disagree")</f>
@@ -7012,7 +7055,7 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B11">
         <f>COUNTIF('Raw Data'!Z$2:Z$17, "Strongly disagree")</f>
@@ -7057,7 +7100,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B12">
         <f>COUNTIF('Raw Data'!AA$2:AA$17, "Strongly disagree")</f>
@@ -7102,7 +7145,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B13">
         <f>COUNTIF('Raw Data'!AB$2:AB$17, "Strongly disagree")</f>
@@ -7147,7 +7190,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -7180,24 +7223,24 @@
         <v>112</v>
       </c>
       <c r="I16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K16" t="s">
+        <v>147</v>
+      </c>
+      <c r="L16" t="s">
         <v>148</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>149</v>
       </c>
-      <c r="M16" t="s">
-        <v>150</v>
-      </c>
       <c r="O16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B17">
         <f>COUNTIF('Raw Data'!AC$2:AC$17, "Strongly disagree")</f>
@@ -7246,7 +7289,7 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B18">
         <f>COUNTIF('Raw Data'!AD$2:AD$17, "Strongly disagree")</f>
@@ -7291,7 +7334,7 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B19">
         <f>COUNTIF('Raw Data'!AE$2:AE$17, "Strongly disagree")</f>
@@ -7336,7 +7379,7 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B20">
         <f>COUNTIF('Raw Data'!AF$2:AF$17, "Strongly disagree")</f>
@@ -7381,7 +7424,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B21">
         <f>COUNTIF('Raw Data'!AG$2:AG$17, "Strongly disagree")</f>
@@ -7426,7 +7469,7 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B22">
         <f>COUNTIF('Raw Data'!AH$2:AH$17, "Strongly disagree")</f>
@@ -7471,7 +7514,7 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B23">
         <f>COUNTIF('Raw Data'!AI$2:AI$17, "Strongly disagree")</f>
@@ -7516,7 +7559,7 @@
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -7549,24 +7592,24 @@
         <v>112</v>
       </c>
       <c r="I27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K27" t="s">
+        <v>147</v>
+      </c>
+      <c r="L27" t="s">
         <v>148</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>149</v>
       </c>
-      <c r="M27" t="s">
-        <v>150</v>
-      </c>
       <c r="O27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B28">
         <f>COUNTIF('Raw Data'!AJ$2:AJ$17, "Strongly disagree")</f>
@@ -7610,12 +7653,12 @@
       </c>
       <c r="O28">
         <f>AVERAGE(M28:M35)</f>
-        <v>3.95</v>
+        <v>3.8444444444444446</v>
       </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B29">
         <f>COUNTIF('Raw Data'!AK$2:AK$17, "Strongly disagree")</f>
@@ -7646,21 +7689,21 @@
         <v>15</v>
       </c>
       <c r="K29">
-        <f t="shared" ref="K29:K31" si="8">B29*1 +C29*2 +D29*3 + E29*4 + F29*5</f>
+        <f t="shared" ref="K29:K30" si="8">B29*1 +C29*2 +D29*3 + E29*4 + F29*5</f>
         <v>59</v>
       </c>
       <c r="L29">
-        <f t="shared" ref="L29:L31" si="9">SUM(B29:F29)</f>
+        <f t="shared" ref="L29:L30" si="9">SUM(B29:F29)</f>
         <v>15</v>
       </c>
       <c r="M29">
-        <f t="shared" ref="M29:M31" si="10">K29/L29</f>
+        <f t="shared" ref="M29:M30" si="10">K29/L29</f>
         <v>3.9333333333333331</v>
       </c>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B30">
         <f>COUNTIF('Raw Data'!AL$2:AL$17, "Strongly disagree")</f>
@@ -7703,56 +7746,79 @@
         <v>3.6666666666666665</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
-      <c r="A31" t="s">
-        <v>147</v>
-      </c>
-      <c r="B31">
+    <row r="36" spans="1:15">
+      <c r="A36" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="O36" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" t="s">
+        <v>146</v>
+      </c>
+      <c r="B37">
         <f>COUNTIF('Raw Data'!AM$2:AM$17, "Strongly disagree")</f>
         <v>0</v>
       </c>
-      <c r="C31">
+      <c r="C37">
         <f>COUNTIF('Raw Data'!AM$2:AM$17, "Disagree")</f>
         <v>0</v>
       </c>
-      <c r="D31">
+      <c r="D37">
         <f>COUNTIF('Raw Data'!AM$2:AM$17, "Neutral")</f>
         <v>2</v>
       </c>
-      <c r="E31">
+      <c r="E37">
         <f>COUNTIF('Raw Data'!AM$2:AM$17, "Agree")</f>
         <v>7</v>
       </c>
-      <c r="F31">
+      <c r="F37">
         <f>COUNTIF('Raw Data'!AM$2:AM$17, "Strongly agree")</f>
         <v>6</v>
       </c>
-      <c r="G31">
+      <c r="G37">
         <f>COUNTIF('Raw Data'!AM$2:AM$17, "Not Applicable")</f>
         <v>0</v>
       </c>
-      <c r="I31">
-        <f>SUM(B31:G31)</f>
-        <v>15</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="8"/>
+      <c r="I37">
+        <f>SUM(B37:G37)</f>
+        <v>15</v>
+      </c>
+      <c r="K37">
+        <f>B37*1 +C37*2 +D37*3 + E37*4 + F37*5</f>
         <v>64</v>
       </c>
-      <c r="L31">
-        <f t="shared" si="9"/>
-        <v>15</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="10"/>
+      <c r="L37">
+        <f>SUM(B37:F37)</f>
+        <v>15</v>
+      </c>
+      <c r="M37">
+        <f>K37/L37</f>
         <v>4.2666666666666666</v>
       </c>
+      <c r="O37">
+        <f>AVERAGE(M6:M37)</f>
+        <v>4.1093111566795786</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A15:K15"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A26:K26"/>
+    <mergeCell ref="A36:K36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated usability survey result 1
</commit_message>
<xml_diff>
--- a/documents/resources/evaluation/usability/Survey-Compiled.xlsx
+++ b/documents/resources/evaluation/usability/Survey-Compiled.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="177">
   <si>
     <t>Male</t>
   </si>
@@ -541,26 +541,29 @@
     <t>Discipline</t>
   </si>
   <si>
-    <t>TOTAL ASQ SCORE</t>
-  </si>
-  <si>
-    <t>ASQ SCORE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Overall, I am satisfied with how easy it is to use this system </t>
   </si>
   <si>
-    <t>OVERALL USABILITY FINAL SCORE</t>
-  </si>
-  <si>
     <t>Overall Usability</t>
+  </si>
+  <si>
+    <t>OVERALL USABILITY FINAL SCORE (Average the 19 questions)</t>
+  </si>
+  <si>
+    <t>Sum Response</t>
+  </si>
+  <si>
+    <t>AVG ASQ SCORE Per Question</t>
+  </si>
+  <si>
+    <t>AVERAGE OVERALL ASQ SCORE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -599,6 +602,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -629,7 +639,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="155">
+  <cellStyleXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -785,8 +795,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -802,8 +834,9 @@
     <xf numFmtId="22" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="155">
+  <cellStyles count="177">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -881,6 +914,17 @@
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -958,6 +1002,17 @@
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3597,7 +3652,7 @@
   <dimension ref="A1:AQ23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AN2" sqref="AN2"/>
+      <selection activeCell="A25" sqref="A25:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5873,8 +5928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L56"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="M49" sqref="M49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6231,12 +6286,12 @@
   <dimension ref="B3:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:E14"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="19.1640625" customWidth="1"/>
     <col min="5" max="6" width="19.83203125" customWidth="1"/>
@@ -6431,7 +6486,7 @@
     </row>
     <row r="11" spans="2:10">
       <c r="B11" t="s">
-        <v>134</v>
+        <v>174</v>
       </c>
       <c r="C11">
         <f>SUM(C4:C9)</f>
@@ -6456,7 +6511,7 @@
     </row>
     <row r="12" spans="2:10">
       <c r="B12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C12">
         <f>(C4*1 +C5*2 +C6* 3 +C7*4 +C8 * 5) /SUM(C4:C8)</f>
@@ -6471,11 +6526,11 @@
         <v>4.2857142857142856</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:10" ht="25">
       <c r="B14" t="s">
-        <v>171</v>
-      </c>
-      <c r="C14">
+        <v>176</v>
+      </c>
+      <c r="C14" s="9">
         <f>AVERAGE(C12:E12)</f>
         <v>4.3619047619047615</v>
       </c>
@@ -6497,12 +6552,12 @@
   <dimension ref="B3:J14"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
@@ -6722,7 +6777,7 @@
     </row>
     <row r="12" spans="2:10">
       <c r="B12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C12">
         <f>(C4*1 +C5*2 +C6* 3 +C7*4 +C8 * 5) /SUM(C4:C8)</f>
@@ -6736,12 +6791,16 @@
         <f t="shared" si="2"/>
         <v>4.2857142857142856</v>
       </c>
-    </row>
-    <row r="14" spans="2:10">
+      <c r="H12">
+        <f>(H4*1 +H5*2 +H6* 3 +H7*4 +H8 * 5) /SUM(H4:H8)</f>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="25">
       <c r="B14" t="s">
-        <v>171</v>
-      </c>
-      <c r="C14">
+        <v>176</v>
+      </c>
+      <c r="C14" s="9">
         <f>AVERAGE(C12:E12)</f>
         <v>4.3841269841269837</v>
       </c>
@@ -6762,8 +6821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6826,7 +6885,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B6">
         <f>COUNTIF('Raw Data'!U$2:U$17, "Strongly disagree")</f>
@@ -7573,36 +7632,6 @@
       <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:15">
-      <c r="B27" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" t="s">
-        <v>112</v>
-      </c>
-      <c r="I27" t="s">
-        <v>134</v>
-      </c>
-      <c r="K27" t="s">
-        <v>147</v>
-      </c>
-      <c r="L27" t="s">
-        <v>148</v>
-      </c>
-      <c r="M27" t="s">
-        <v>149</v>
-      </c>
       <c r="O27" t="s">
         <v>152</v>
       </c>
@@ -7746,22 +7775,54 @@
         <v>3.6666666666666665</v>
       </c>
     </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+    </row>
     <row r="36" spans="1:15">
-      <c r="A36" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" t="s">
+        <v>112</v>
+      </c>
+      <c r="I36" t="s">
+        <v>134</v>
+      </c>
+      <c r="K36" t="s">
+        <v>147</v>
+      </c>
+      <c r="L36" t="s">
+        <v>148</v>
+      </c>
+      <c r="M36" t="s">
+        <v>149</v>
+      </c>
       <c r="O36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:15">
@@ -7818,7 +7879,7 @@
     <mergeCell ref="A15:K15"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A26:K26"/>
-    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A35:K35"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>